<commit_message>
final dataset, removed spaces, nan handling
</commit_message>
<xml_diff>
--- a/AuctionData.xlsx
+++ b/AuctionData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abm/Desktop/IPL-Bidding/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61D3E47B-AFA0-9F47-A7B0-5817DD518610}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46726DC1-3335-0045-91BC-77990B07D6F1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="20800" windowHeight="12320" xr2:uid="{9FA3F907-E0DB-4834-A317-9BDD54F32D38}"/>
   </bookViews>
@@ -249,7 +249,7 @@
     <t xml:space="preserve"> Chennai Super Kings</t>
   </si>
   <si>
-    <t xml:space="preserve"> Delhi</t>
+    <t xml:space="preserve"> Delhi Capitals</t>
   </si>
 </sst>
 </file>
@@ -618,8 +618,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:E66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B67" sqref="B67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>